<commit_message>
Création d'un HTML, CSS et Javascripts
</commit_message>
<xml_diff>
--- a/Diagramme/ExcelDiagramme.xlsx
+++ b/Diagramme/ExcelDiagramme.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Desktop\Cegep\Session 3\Projet Long BD2\Diagramme\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Desktop\Cegep\Session 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{056447A4-12D8-44AE-A214-1ECCFA2024EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF13BED0-88CB-4B2D-8A60-FF0BFE0442A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22C69845-49B9-4148-8E6F-39FFDFA9FA58}"/>
   </bookViews>
@@ -36,16 +36,61 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
   <si>
     <t>Clients</t>
+  </si>
+  <si>
+    <t>Nom</t>
+  </si>
+  <si>
+    <t>Cellulaire</t>
+  </si>
+  <si>
+    <t>Addresse</t>
+  </si>
+  <si>
+    <t>Code Postal</t>
+  </si>
+  <si>
+    <t>Province</t>
+  </si>
+  <si>
+    <t>Pays</t>
+  </si>
+  <si>
+    <t>Ville</t>
+  </si>
+  <si>
+    <t>Commande</t>
+  </si>
+  <si>
+    <t>Croute</t>
+  </si>
+  <si>
+    <t>Sauce</t>
+  </si>
+  <si>
+    <t>Garniture</t>
+  </si>
+  <si>
+    <t>Prix</t>
+  </si>
+  <si>
+    <t>Commande Attente</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Taille</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -410,17 +455,115 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A94FA77-ABE0-4992-A5F9-BB024562D3AE}">
-  <dimension ref="C3"/>
+  <dimension ref="C3:O11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="3:3">
+    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>10</v>
+      </c>
+      <c r="M3" t="s">
+        <v>15</v>
+      </c>
+      <c r="O3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>1</v>
+      </c>
+      <c r="K5" t="s">
+        <v>1</v>
+      </c>
+      <c r="M5" t="s">
+        <v>1</v>
+      </c>
+      <c r="O5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I6" t="s">
+        <v>12</v>
+      </c>
+      <c r="K6" t="s">
+        <v>12</v>
+      </c>
+      <c r="M6" t="s">
+        <v>12</v>
+      </c>
+      <c r="O6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ajout du Scripts de SQL
</commit_message>
<xml_diff>
--- a/Diagramme/ExcelDiagramme.xlsx
+++ b/Diagramme/ExcelDiagramme.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\Desktop\Cegep\Session 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\willi\OneDrive\Bureau\Cegep\Session 3\BD2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F5D545-656E-4D43-98A1-47185935332B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9ED11C3F-42BC-4DA3-8606-C3BDEF832D3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22C69845-49B9-4148-8E6F-39FFDFA9FA58}"/>
+    <workbookView xWindow="-96" yWindow="0" windowWidth="8748" windowHeight="12336" xr2:uid="{22C69845-49B9-4148-8E6F-39FFDFA9FA58}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>Clients</t>
   </si>
@@ -74,16 +74,13 @@
     <t>Garniture</t>
   </si>
   <si>
-    <t>Prix</t>
-  </si>
-  <si>
     <t>Commande Attente</t>
   </si>
   <si>
     <t>Client</t>
   </si>
   <si>
-    <t>Taille</t>
+    <t>Garniture_Commande</t>
   </si>
 </sst>
 </file>
@@ -455,15 +452,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A94FA77-ABE0-4992-A5F9-BB024562D3AE}">
-  <dimension ref="C3:O11"/>
+  <dimension ref="C3:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q8" sqref="Q8"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="3" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C3" t="s">
         <v>0</v>
       </c>
@@ -480,13 +477,10 @@
         <v>10</v>
       </c>
       <c r="M3" t="s">
-        <v>15</v>
-      </c>
-      <c r="O3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="3:15" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C5" t="s">
         <v>1</v>
       </c>
@@ -503,36 +497,21 @@
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>1</v>
-      </c>
-      <c r="O5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="3:15" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C6" t="s">
         <v>2</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
       </c>
-      <c r="G6" t="s">
-        <v>12</v>
-      </c>
-      <c r="I6" t="s">
-        <v>12</v>
-      </c>
-      <c r="K6" t="s">
-        <v>12</v>
-      </c>
       <c r="M6" t="s">
-        <v>12</v>
-      </c>
-      <c r="O6" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>3</v>
       </c>
@@ -540,30 +519,36 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C8" t="s">
         <v>7</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="3:15" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>5</v>
       </c>
-      <c r="E9" t="s">
+      <c r="I9" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="3:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="11" spans="3:15" x14ac:dyDescent="0.25">
+      <c r="I10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="3:13" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>4</v>
+      </c>
+      <c r="I11" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>